<commit_message>
fixed some errors and the graph
</commit_message>
<xml_diff>
--- a/graph-throughput-vs-loss.xlsx
+++ b/graph-throughput-vs-loss.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="80" windowWidth="20000" windowHeight="12080" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="740" yWindow="80" windowWidth="24600" windowHeight="15120" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -137,7 +137,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -166,7 +165,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -236,11 +234,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2066152136"/>
-        <c:axId val="2066155224"/>
+        <c:axId val="2078256824"/>
+        <c:axId val="2038637464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2066152136"/>
+        <c:axId val="2078256824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -262,14 +260,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066155224"/>
+        <c:crossAx val="2038637464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -277,7 +274,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2066155224"/>
+        <c:axId val="2038637464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -300,14 +297,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066152136"/>
+        <c:crossAx val="2078256824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -482,11 +478,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2146577752"/>
-        <c:axId val="-2146579800"/>
+        <c:axId val="2074335736"/>
+        <c:axId val="2074341240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2146577752"/>
+        <c:axId val="2074335736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,7 +511,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146579800"/>
+        <c:crossAx val="2074341240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -523,7 +519,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2146579800"/>
+        <c:axId val="2074341240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,7 +549,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146577752"/>
+        <c:crossAx val="2074335736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -562,6 +558,13 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -610,15 +613,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1031,7 +1034,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>